<commit_message>
добавила TestCase i Description_2
</commit_message>
<xml_diff>
--- a/test_case/TestCase.xlsx
+++ b/test_case/TestCase.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Identefier</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Ввод  нового номера телефона и получение кода для подтверждения</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>Steps</t>
   </si>
 </sst>
 </file>
@@ -298,7 +304,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,14 +339,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -368,6 +368,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:K13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,8 +706,8 @@
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="4">
-        <v>2</v>
+      <c r="G1" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -717,7 +723,7 @@
       <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -725,15 +731,15 @@
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="8"/>
@@ -748,11 +754,11 @@
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="27"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="2"/>
       <c r="M3" s="10"/>
       <c r="N3" s="11"/>
@@ -767,11 +773,11 @@
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="27"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="2"/>
       <c r="M4" s="10"/>
       <c r="N4" s="11"/>
@@ -783,16 +789,16 @@
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="27"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
       <c r="L5" s="2"/>
       <c r="M5" s="10"/>
       <c r="N5" s="11"/>
@@ -801,19 +807,19 @@
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="2"/>
       <c r="M6" s="10"/>
       <c r="N6" s="11"/>
@@ -822,17 +828,17 @@
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
       <c r="L7" s="2"/>
       <c r="M7" s="10"/>
       <c r="N7" s="11"/>
@@ -841,17 +847,17 @@
       <c r="Q7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="2"/>
       <c r="M8" s="10"/>
       <c r="N8" s="11"/>
@@ -860,17 +866,17 @@
       <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="2"/>
       <c r="M9" s="10"/>
       <c r="N9" s="11"/>
@@ -885,11 +891,11 @@
       <c r="D10" s="17"/>
       <c r="E10" s="18"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
       <c r="L10" s="2"/>
       <c r="M10" s="10"/>
       <c r="N10" s="11"/>
@@ -906,11 +912,11 @@
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
       <c r="L11" s="2"/>
       <c r="M11" s="13"/>
       <c r="N11" s="14"/>
@@ -919,13 +925,13 @@
       <c r="Q11" s="15"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="2"/>
       <c r="G12" s="16"/>
       <c r="H12" s="17"/>
@@ -940,11 +946,11 @@
       <c r="Q12" s="18"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
       <c r="F13" s="2"/>
       <c r="G13" s="4" t="s">
         <v>4</v>
@@ -963,19 +969,19 @@
       <c r="Q13" s="6"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="9"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="7"/>
+      <c r="M14" s="19"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
@@ -1022,7 +1028,9 @@
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1085,11 +1093,6 @@
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A17:E19"/>
     <mergeCell ref="F1:F19"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G2:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K19"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A6:E9"/>
@@ -1097,6 +1100,11 @@
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E14"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G2:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K19"/>
     <mergeCell ref="L1:L19"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="M2:Q11"/>

</xml_diff>